<commit_message>
Updated EOL for 11.2 and 11.3
</commit_message>
<xml_diff>
--- a/doc/container_tags.xlsx
+++ b/doc/container_tags.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nvidia-my.sharepoint.com/personal/srivatsans_nvidia_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40B4A7B9-7995-42CB-90B5-47711A6F39F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{40B4A7B9-7995-42CB-90B5-47711A6F39F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D05D75D-55F1-4A25-A9B8-EA2D47D34B46}"/>
   <bookViews>
-    <workbookView xWindow="1226" yWindow="-103" windowWidth="31791" windowHeight="18720" xr2:uid="{5ADAA6C5-3FC4-485E-AC2B-0526B6C75DBB}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{5ADAA6C5-3FC4-485E-AC2B-0526B6C75DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="39">
   <si>
     <t>v11.2.0</t>
   </si>
@@ -151,6 +150,9 @@
   </si>
   <si>
     <t>CUDA Container Tag Support EOL Chart</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -158,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -236,13 +238,10 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -255,6 +254,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -573,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F174569B-432C-4AEF-8100-B12D045F7A7D}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -585,514 +587,536 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>44927</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>45047</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>45108</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>45261</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>45474</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>510</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>515</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>450</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>525</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>45200</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>45200</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>45078</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>45078</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>45078</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>45078</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>45078</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>45078</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>45078</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>45078</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="B24" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>45078</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B27" s="3">
         <v>45078</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="3">
         <v>45078</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="B29" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="B30" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>

</xml_diff>